<commit_message>
CARGA DE DATOS INTEGRADA
</commit_message>
<xml_diff>
--- a/src/test/resources/prueba.xlsx
+++ b/src/test/resources/prueba.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="198">
   <si>
     <t>Legajo</t>
   </si>
@@ -610,9 +610,6 @@
   </si>
   <si>
     <t>RODRIGO EZEQUIEL</t>
-  </si>
-  <si>
-    <t>Metodología de la Investigación</t>
   </si>
 </sst>
 </file>
@@ -954,7 +951,7 @@
   <dimension ref="A1:CW51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -976,7 +973,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>198</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>

</xml_diff>